<commit_message>
Newer version fireball test
</commit_message>
<xml_diff>
--- a/Fireball Test.xlsx
+++ b/Fireball Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="S22" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
   <si>
     <t>2-pyridoxine 2-aminopyridine complex</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>This means the results is close to the reference.</t>
+  </si>
+  <si>
+    <t>Fireball test2</t>
   </si>
 </sst>
 </file>
@@ -592,20 +595,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K4" sqref="K4"/>
+      <selection pane="topRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="56.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -627,7 +631,9 @@
       <c r="F1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="H1" s="3" t="s">
         <v>33</v>
       </c>
@@ -708,7 +714,9 @@
       <c r="J4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
       <c r="A5" s="4" t="s">
@@ -737,7 +745,9 @@
       <c r="J5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickTop="1">
       <c r="A6" s="4" t="s">
@@ -766,7 +776,9 @@
       <c r="J6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
@@ -824,7 +836,9 @@
       <c r="J8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
@@ -1323,7 +1337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>

<commit_message>
New paper of fireball added
</commit_message>
<xml_diff>
--- a/Fireball Test.xlsx
+++ b/Fireball Test.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="17250" windowHeight="6885"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="17250" windowHeight="6885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="S22" sheetId="1" r:id="rId1"/>
-    <sheet name="S66" sheetId="2" r:id="rId2"/>
+    <sheet name="H2O CH4" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'S22'!$I$1:$I$26</definedName>
@@ -280,1214 +280,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'S22'!$A$3:$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>Water dimer</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ammonia dimer</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Formic acid dimer</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Formamide dimer</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Uracil dimer h-bonded</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2-pyridoxine 2-aminopyridine complex</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Adenine thymine Watson-Crick complex</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>With predominant dispersion contribution</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Methane dimer</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ethene dimer</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Benzene - Methane complex</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Benzene dimer parallel displaced</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Pyrazine dimer</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Uracil dimer stack</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Indole benzene complex stack</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Adenine thymine complex stack</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Mixed complexes</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Ethene ethyne complex</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Benzene water complex</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Benzene ammonia complex</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Benzene HCN complex</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Benzene dimer T-shaped</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Indole benzene T-shape complex</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Phenol dimer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'S22'!$D$3:$D$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>-5.0199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-3.17</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-18.61</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-15.96</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-20.47</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-16.71</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-16.37</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.53</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1.51</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-1.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-2.73</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-4.42</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-9.8800000000000008</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-5.22</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-12.23</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-1.53</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-3.28</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-2.35</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-4.46</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-2.74</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-5.73</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-7.05</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'S22'!$A$3:$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>Water dimer</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ammonia dimer</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Formic acid dimer</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Formamide dimer</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Uracil dimer h-bonded</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2-pyridoxine 2-aminopyridine complex</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Adenine thymine Watson-Crick complex</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>With predominant dispersion contribution</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Methane dimer</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ethene dimer</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Benzene - Methane complex</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Benzene dimer parallel displaced</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Pyrazine dimer</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Uracil dimer stack</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Indole benzene complex stack</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Adenine thymine complex stack</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Mixed complexes</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Ethene ethyne complex</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Benzene water complex</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Benzene ammonia complex</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Benzene HCN complex</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Benzene dimer T-shaped</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Indole benzene T-shape complex</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Phenol dimer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'S22'!$E$3:$E$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>-5.03</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-3.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-18.600000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-15.86</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-20.43</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-17.37</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-16.54</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.51</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1.62</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-1.86</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-4.95</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-6.9</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-11.15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-8.1199999999999992</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-14.93</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-1.69</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-3.61</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-2.72</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-5.16</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-3.62</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-7.03</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-7.76</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'S22'!$A$3:$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>Water dimer</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ammonia dimer</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Formic acid dimer</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Formamide dimer</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Uracil dimer h-bonded</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2-pyridoxine 2-aminopyridine complex</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Adenine thymine Watson-Crick complex</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>With predominant dispersion contribution</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Methane dimer</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ethene dimer</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Benzene - Methane complex</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Benzene dimer parallel displaced</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Pyrazine dimer</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Uracil dimer stack</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Indole benzene complex stack</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Adenine thymine complex stack</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Mixed complexes</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Ethene ethyne complex</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Benzene water complex</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Benzene ammonia complex</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Benzene HCN complex</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Benzene dimer T-shaped</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Indole benzene T-shape complex</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Phenol dimer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'S22'!$H$3:$H$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>-9.18678036009225</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-4.5121390128299206</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-41.908545214292189</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-31.470762795480169</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-36.981151386665658</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-36.591959652836366</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-33.456275691775005</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.90664482926968781</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-4.0099405382696656</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-2.6117325064210815</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-6.6768879969905566</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-8.7721594921799291</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-16.21724560493054</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-9.9283626227116937</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-22.50893949245911</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-3.7635833344191276</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-9.7402987840495641</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-5.3596545156587228</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-6.3221090404207301</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-5.0098657288800093</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-10.001699600645065</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-16.75237426505868</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="50787072"/>
-        <c:axId val="51202304"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="50787072"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51202304"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="51202304"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50787072"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'S22'!$A$3:$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>Water dimer</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ammonia dimer</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Formic acid dimer</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Formamide dimer</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Uracil dimer h-bonded</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2-pyridoxine 2-aminopyridine complex</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Adenine thymine Watson-Crick complex</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>With predominant dispersion contribution</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Methane dimer</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ethene dimer</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Benzene - Methane complex</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Benzene dimer parallel displaced</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Pyrazine dimer</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Uracil dimer stack</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Indole benzene complex stack</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Adenine thymine complex stack</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Mixed complexes</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Ethene ethyne complex</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Benzene water complex</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Benzene ammonia complex</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Benzene HCN complex</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Benzene dimer T-shaped</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Indole benzene T-shape complex</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Phenol dimer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'S22'!$D$3:$D$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>-5.0199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-3.17</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-18.61</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-15.96</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-20.47</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-16.71</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-16.37</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.53</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1.51</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-1.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-2.73</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-4.42</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-9.8800000000000008</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-5.22</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-12.23</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-1.53</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-3.28</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-2.35</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-4.46</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-2.74</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-5.73</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-7.05</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'S22'!$A$3:$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>Water dimer</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ammonia dimer</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Formic acid dimer</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Formamide dimer</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Uracil dimer h-bonded</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2-pyridoxine 2-aminopyridine complex</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Adenine thymine Watson-Crick complex</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>With predominant dispersion contribution</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Methane dimer</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ethene dimer</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Benzene - Methane complex</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Benzene dimer parallel displaced</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Pyrazine dimer</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Uracil dimer stack</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Indole benzene complex stack</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Adenine thymine complex stack</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Mixed complexes</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Ethene ethyne complex</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Benzene water complex</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Benzene ammonia complex</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Benzene HCN complex</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Benzene dimer T-shaped</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Indole benzene T-shape complex</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Phenol dimer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'S22'!$E$3:$E$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>-5.03</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-3.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-18.600000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-15.86</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-20.43</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-17.37</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-16.54</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.51</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1.62</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-1.86</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-4.95</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-6.9</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-11.15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-8.1199999999999992</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-14.93</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-1.69</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-3.61</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-2.72</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-5.16</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-3.62</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-7.03</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-7.76</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'S22'!$A$3:$A$26</c:f>
-              <c:strCache>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>Water dimer</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Ammonia dimer</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Formic acid dimer</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Formamide dimer</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Uracil dimer h-bonded</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2-pyridoxine 2-aminopyridine complex</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Adenine thymine Watson-Crick complex</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>With predominant dispersion contribution</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Methane dimer</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Ethene dimer</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Benzene - Methane complex</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Benzene dimer parallel displaced</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Pyrazine dimer</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Uracil dimer stack</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Indole benzene complex stack</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Adenine thymine complex stack</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Mixed complexes</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Ethene ethyne complex</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Benzene water complex</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Benzene ammonia complex</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Benzene HCN complex</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Benzene dimer T-shaped</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Indole benzene T-shape complex</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Phenol dimer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'S22'!$K$3:$K$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
-                <c:pt idx="0">
-                  <c:v>-11.408646367831459</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-6.1548609827984277</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-47.554003696743521</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-35.221653355499093</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-42.629668218935414</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-41.839631566777754</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-39.423928399033258</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-5.8646585914800742</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-3.6729699777310461</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.11903327186753461</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-9.6486744331138627</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-11.809572691499344</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-20.580881693995757</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-14.122032915298492</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-3.2794953549885304</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-12.998035163098551</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-10.997499870177235</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-5.810299663497684</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-4.3209148947311036</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-9.285475674832302</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-21.413256958500774</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="52672768"/>
-        <c:axId val="52682752"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="52672768"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52682752"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="52682752"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52672768"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1057275</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1745,7 +537,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1755,9 +547,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K38" sqref="K38"/>
+      <selection pane="topRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1860,7 +652,7 @@
         <v>-0.49471603000006326</v>
       </c>
       <c r="K3" s="1">
-        <f>J3*23.061</f>
+        <f t="shared" ref="K3:K9" si="0">J3*23.061</f>
         <v>-11.408646367831459</v>
       </c>
     </row>
@@ -1888,7 +680,7 @@
         <v>-0.19566102999999657</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H26" si="0">G4*23.061</f>
+        <f t="shared" ref="H4:H26" si="1">G4*23.061</f>
         <v>-4.5121390128299206</v>
       </c>
       <c r="I4" s="1">
@@ -1899,7 +691,7 @@
         <v>-0.26689479999993182</v>
       </c>
       <c r="K4" s="1">
-        <f>J4*23.061</f>
+        <f t="shared" si="0"/>
         <v>-6.1548609827984277</v>
       </c>
     </row>
@@ -1927,7 +719,7 @@
         <v>-1.8172908900000948</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-41.908545214292189</v>
       </c>
       <c r="I5" s="1">
@@ -1938,7 +730,7 @@
         <v>-2.0620963400001528</v>
       </c>
       <c r="K5" s="1">
-        <f>J5*23.061</f>
+        <f t="shared" si="0"/>
         <v>-47.554003696743521</v>
       </c>
     </row>
@@ -1966,7 +758,7 @@
         <v>-1.3646746800000074</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-31.470762795480169</v>
       </c>
       <c r="I6" s="1">
@@ -1977,7 +769,7 @@
         <v>-1.5273254999999608</v>
       </c>
       <c r="K6" s="1">
-        <f>J6*23.061</f>
+        <f t="shared" si="0"/>
         <v>-35.221653355499093</v>
       </c>
     </row>
@@ -2005,7 +797,7 @@
         <v>-1.6036230600002455</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-36.981151386665658</v>
       </c>
       <c r="I7" s="1">
@@ -2016,7 +808,7 @@
         <v>-1.8485611300002347</v>
       </c>
       <c r="K7" s="1">
-        <f>J7*23.061</f>
+        <f t="shared" si="0"/>
         <v>-42.629668218935414</v>
       </c>
     </row>
@@ -2044,7 +836,7 @@
         <v>-1.5867464399998426</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-36.591959652836366</v>
       </c>
       <c r="I8" s="1">
@@ -2055,7 +847,7 @@
         <v>-1.8143025700003363</v>
       </c>
       <c r="K8" s="1">
-        <f>J8*23.061</f>
+        <f t="shared" si="0"/>
         <v>-41.839631566777754</v>
       </c>
     </row>
@@ -2083,7 +875,7 @@
         <v>-1.4507729799997833</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-33.456275691775005</v>
       </c>
       <c r="I9" s="1">
@@ -2094,7 +886,7 @@
         <v>-1.709549820000575</v>
       </c>
       <c r="K9" s="1">
-        <f>J9*23.061</f>
+        <f t="shared" si="0"/>
         <v>-39.423928399033258</v>
       </c>
     </row>
@@ -2137,7 +929,7 @@
         <v>-3.9315069999986463E-2</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.90664482926968781</v>
       </c>
       <c r="I11" s="1">
@@ -2148,7 +940,7 @@
         <v>-0.25431068000000323</v>
       </c>
       <c r="K11" s="1">
-        <f>J11*23.061</f>
+        <f t="shared" ref="K11:K17" si="2">J11*23.061</f>
         <v>-5.8646585914800742</v>
       </c>
     </row>
@@ -2176,7 +968,7 @@
         <v>-0.17388406999998551</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4.0099405382696656</v>
       </c>
       <c r="I12" s="1">
@@ -2187,7 +979,7 @@
         <v>-0.15927193000004536</v>
       </c>
       <c r="K12" s="1">
-        <f>J12*23.061</f>
+        <f t="shared" si="2"/>
         <v>-3.6729699777310461</v>
       </c>
     </row>
@@ -2215,7 +1007,7 @@
         <v>-0.11325322000004689</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.6117325064210815</v>
       </c>
       <c r="I13" s="1">
@@ -2226,7 +1018,7 @@
         <v>-5.1616699998930926E-3</v>
       </c>
       <c r="K13" s="1">
-        <f>J13*23.061</f>
+        <f t="shared" si="2"/>
         <v>-0.11903327186753461</v>
       </c>
     </row>
@@ -2254,7 +1046,7 @@
         <v>-0.28953159000002415</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6.6768879969905566</v>
       </c>
       <c r="I14" s="1">
@@ -2265,7 +1057,7 @@
         <v>-0.41839791999973386</v>
       </c>
       <c r="K14" s="1">
-        <f>J14*23.061</f>
+        <f t="shared" si="2"/>
         <v>-9.6486744331138627</v>
       </c>
     </row>
@@ -2293,7 +1085,7 @@
         <v>-0.38038937999999689</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-8.7721594921799291</v>
       </c>
       <c r="I15" s="1">
@@ -2304,7 +1096,7 @@
         <v>-0.51210149999997157</v>
       </c>
       <c r="K15" s="1">
-        <f>J15*23.061</f>
+        <f t="shared" si="2"/>
         <v>-11.809572691499344</v>
       </c>
     </row>
@@ -2332,7 +1124,7 @@
         <v>-0.70323253999958979</v>
       </c>
       <c r="H16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-16.21724560493054</v>
       </c>
       <c r="I16" s="1">
@@ -2343,7 +1135,7 @@
         <v>-0.89245399999981601</v>
       </c>
       <c r="K16" s="1">
-        <f>J16*23.061</f>
+        <f t="shared" si="2"/>
         <v>-20.580881693995757</v>
       </c>
     </row>
@@ -2371,7 +1163,7 @@
         <v>-0.43052611000007346</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9.9283626227116937</v>
       </c>
       <c r="I17" s="1">
@@ -2382,7 +1174,7 @@
         <v>-0.61237729999993462</v>
       </c>
       <c r="K17" s="1">
-        <f>J17*23.061</f>
+        <f t="shared" si="2"/>
         <v>-14.122032915298492</v>
       </c>
     </row>
@@ -2410,12 +1202,20 @@
         <v>-0.97606085999996139</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-22.50893949245911</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="I18" s="1">
+        <v>-4493.5458151299999</v>
+      </c>
+      <c r="J18" s="1">
+        <f>I18-I30-I42</f>
+        <v>-1.273630470000171</v>
+      </c>
+      <c r="K18" s="1">
+        <f>J18*23.061</f>
+        <v>-29.371192268673944</v>
+      </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="2" t="s">
@@ -2456,7 +1256,7 @@
         <v>-0.16320121999996218</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.7635833344191276</v>
       </c>
       <c r="I20" s="1">
@@ -2467,7 +1267,7 @@
         <v>-0.14220958999993627</v>
       </c>
       <c r="K20" s="1">
-        <f>J20*23.061</f>
+        <f t="shared" ref="K20:K26" si="3">J20*23.061</f>
         <v>-3.2794953549885304</v>
       </c>
     </row>
@@ -2495,7 +1295,7 @@
         <v>-0.4223710499999811</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9.7402987840495641</v>
       </c>
       <c r="I21" s="1">
@@ -2506,7 +1306,7 @@
         <v>-0.56363709999993716</v>
       </c>
       <c r="K21" s="1">
-        <f>J21*23.061</f>
+        <f t="shared" si="3"/>
         <v>-12.998035163098551</v>
       </c>
     </row>
@@ -2534,7 +1334,7 @@
         <v>-0.23241205999994463</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-5.3596545156587228</v>
       </c>
       <c r="I22" s="1">
@@ -2545,7 +1345,7 @@
         <v>-0.47688737999988007</v>
       </c>
       <c r="K22" s="1">
-        <f>J22*23.061</f>
+        <f t="shared" si="3"/>
         <v>-10.997499870177235</v>
       </c>
     </row>
@@ -2573,7 +1373,7 @@
         <v>-0.27414722000003167</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-6.3221090404207301</v>
       </c>
       <c r="I23" s="1">
@@ -2584,7 +1384,7 @@
         <v>-0.25195349999989958</v>
       </c>
       <c r="K23" s="1">
-        <f>J23*23.061</f>
+        <f t="shared" si="3"/>
         <v>-5.810299663497684</v>
       </c>
     </row>
@@ -2612,7 +1412,7 @@
         <v>-0.21724408000000039</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-5.0098657288800093</v>
       </c>
       <c r="I24" s="1">
@@ -2623,7 +1423,7 @@
         <v>-0.18736893000004784</v>
       </c>
       <c r="K24" s="1">
-        <f>J24*23.061</f>
+        <f t="shared" si="3"/>
         <v>-4.3209148947311036</v>
       </c>
     </row>
@@ -2651,7 +1451,7 @@
         <v>-0.43370624000021962</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-10.001699600645065</v>
       </c>
       <c r="I25" s="1">
@@ -2662,7 +1462,7 @@
         <v>-0.40264843999966615</v>
       </c>
       <c r="K25" s="1">
-        <f>J25*23.061</f>
+        <f t="shared" si="3"/>
         <v>-9.285475674832302</v>
       </c>
     </row>
@@ -2690,7 +1490,7 @@
         <v>-0.7264374599999428</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-16.75237426505868</v>
       </c>
       <c r="I26" s="1">
@@ -2701,7 +1501,7 @@
         <v>-0.92854850000003353</v>
       </c>
       <c r="K26" s="1">
-        <f>J26*23.061</f>
+        <f t="shared" si="3"/>
         <v>-21.413256958500774</v>
       </c>
     </row>
@@ -3055,7 +1855,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3063,11 +1862,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>